<commit_message>
#85 added extra metacore comment and updated specs to include ACTARM ready for AE table example
</commit_message>
<xml_diff>
--- a/metadata/safety_specs.xlsx
+++ b/metadata/safety_specs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38352" windowHeight="19992" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38352" windowHeight="19992" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="694">
   <si>
     <t>Attribute</t>
   </si>
@@ -2197,6 +2197,9 @@
   </si>
   <si>
     <t>Set to the SMQ name if the AE term matches any term within this AE query.</t>
+  </si>
+  <si>
+    <t>ADSL.ACTARM</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -2980,13 +2983,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R163"/>
+  <dimension ref="A1:R164"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D110" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C160" sqref="C160"/>
+      <selection pane="bottomRight" activeCell="M140" sqref="M140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7803,7 +7806,7 @@
       <c r="O128"/>
       <c r="P128"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="13">
         <v>8</v>
       </c>
@@ -7839,7 +7842,7 @@
       <c r="O129"/>
       <c r="P129"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="13">
         <v>9</v>
       </c>
@@ -7875,7 +7878,7 @@
       <c r="O130"/>
       <c r="P130"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="13">
         <v>10</v>
       </c>
@@ -7913,7 +7916,7 @@
       <c r="O131"/>
       <c r="P131"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="13">
         <v>11</v>
       </c>
@@ -7951,7 +7954,7 @@
       <c r="O132"/>
       <c r="P132"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="13">
         <v>12</v>
       </c>
@@ -7989,7 +7992,7 @@
       <c r="O133"/>
       <c r="P133"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="13">
         <v>13</v>
       </c>
@@ -8011,7 +8014,7 @@
       <c r="G134"/>
       <c r="H134" s="13"/>
       <c r="I134" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J134" t="s">
         <v>265</v>
@@ -8027,7 +8030,7 @@
       <c r="O134"/>
       <c r="P134"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="13">
         <v>14</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>126</v>
       </c>
       <c r="I135" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J135"/>
       <c r="K135" t="s">
@@ -8065,7 +8068,7 @@
       <c r="O135"/>
       <c r="P135"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="13">
         <v>15</v>
       </c>
@@ -8089,7 +8092,7 @@
         <v>133</v>
       </c>
       <c r="I136" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J136"/>
       <c r="K136" t="s">
@@ -8103,7 +8106,7 @@
       <c r="O136"/>
       <c r="P136"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" s="13">
         <v>16</v>
       </c>
@@ -8127,7 +8130,7 @@
         <v>126</v>
       </c>
       <c r="I137" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J137"/>
       <c r="K137" t="s">
@@ -8141,7 +8144,7 @@
       <c r="O137"/>
       <c r="P137"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" s="13">
         <v>17</v>
       </c>
@@ -8163,7 +8166,7 @@
       <c r="G138"/>
       <c r="H138" s="13"/>
       <c r="I138" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J138"/>
       <c r="K138" t="s">
@@ -8177,7 +8180,7 @@
       <c r="O138"/>
       <c r="P138"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" s="13">
         <v>18</v>
       </c>
@@ -8201,7 +8204,7 @@
         <v>126</v>
       </c>
       <c r="I139" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J139"/>
       <c r="K139" t="s">
@@ -8215,7 +8218,7 @@
       <c r="O139"/>
       <c r="P139"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="13">
         <v>19</v>
       </c>
@@ -8223,35 +8226,36 @@
         <v>607</v>
       </c>
       <c r="C140" t="s">
-        <v>649</v>
+        <v>66</v>
       </c>
       <c r="D140" t="s">
-        <v>342</v>
+        <v>82</v>
       </c>
       <c r="E140" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="F140">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G140"/>
-      <c r="H140" s="13"/>
       <c r="I140" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J140"/>
       <c r="K140" t="s">
         <v>23</v>
       </c>
       <c r="L140"/>
-      <c r="M140" s="11"/>
+      <c r="M140"/>
       <c r="N140" t="s">
-        <v>681</v>
+        <v>693</v>
       </c>
       <c r="O140"/>
       <c r="P140"/>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q140"/>
+      <c r="R140"/>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" s="13">
         <v>20</v>
       </c>
@@ -8259,16 +8263,16 @@
         <v>607</v>
       </c>
       <c r="C141" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D141" t="s">
-        <v>680</v>
+        <v>342</v>
       </c>
       <c r="E141" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="F141">
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="G141"/>
       <c r="H141" s="13"/>
@@ -8282,12 +8286,12 @@
       <c r="L141"/>
       <c r="M141" s="11"/>
       <c r="N141" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="O141"/>
       <c r="P141"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142" s="13">
         <v>21</v>
       </c>
@@ -8295,10 +8299,10 @@
         <v>607</v>
       </c>
       <c r="C142" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D142" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E142" t="s">
         <v>84</v>
@@ -8318,12 +8322,12 @@
       <c r="L142"/>
       <c r="M142" s="11"/>
       <c r="N142" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="O142"/>
       <c r="P142"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" s="13">
         <v>22</v>
       </c>
@@ -8331,16 +8335,16 @@
         <v>607</v>
       </c>
       <c r="C143" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D143" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E143" t="s">
         <v>84</v>
       </c>
       <c r="F143">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="G143"/>
       <c r="H143" s="13"/>
@@ -8354,12 +8358,12 @@
       <c r="L143"/>
       <c r="M143" s="11"/>
       <c r="N143" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="O143"/>
       <c r="P143"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="13">
         <v>23</v>
       </c>
@@ -8367,16 +8371,16 @@
         <v>607</v>
       </c>
       <c r="C144" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D144" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E144" t="s">
         <v>84</v>
       </c>
       <c r="F144">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="G144"/>
       <c r="H144" s="13"/>
@@ -8390,7 +8394,7 @@
       <c r="L144"/>
       <c r="M144" s="11"/>
       <c r="N144" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="O144"/>
       <c r="P144"/>
@@ -8403,16 +8407,16 @@
         <v>607</v>
       </c>
       <c r="C145" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D145" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="E145" t="s">
         <v>84</v>
       </c>
       <c r="F145">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="G145"/>
       <c r="H145" s="13"/>
@@ -8426,7 +8430,7 @@
       <c r="L145"/>
       <c r="M145" s="11"/>
       <c r="N145" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O145"/>
       <c r="P145"/>
@@ -8439,10 +8443,10 @@
         <v>607</v>
       </c>
       <c r="C146" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D146" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E146" t="s">
         <v>84</v>
@@ -8462,7 +8466,7 @@
       <c r="L146"/>
       <c r="M146" s="11"/>
       <c r="N146" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="O146"/>
       <c r="P146"/>
@@ -8475,10 +8479,10 @@
         <v>607</v>
       </c>
       <c r="C147" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D147" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E147" t="s">
         <v>84</v>
@@ -8498,7 +8502,7 @@
       <c r="L147"/>
       <c r="M147" s="11"/>
       <c r="N147" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="O147"/>
       <c r="P147"/>
@@ -8511,16 +8515,16 @@
         <v>607</v>
       </c>
       <c r="C148" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D148" t="s">
-        <v>659</v>
+        <v>674</v>
       </c>
       <c r="E148" t="s">
         <v>84</v>
       </c>
       <c r="F148">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="G148"/>
       <c r="H148" s="13"/>
@@ -8534,7 +8538,7 @@
       <c r="L148"/>
       <c r="M148" s="11"/>
       <c r="N148" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="O148"/>
       <c r="P148"/>
@@ -8547,10 +8551,10 @@
         <v>607</v>
       </c>
       <c r="C149" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D149" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E149" t="s">
         <v>84</v>
@@ -8570,7 +8574,7 @@
       <c r="L149"/>
       <c r="M149" s="11"/>
       <c r="N149" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="O149"/>
       <c r="P149"/>
@@ -8582,31 +8586,34 @@
       <c r="B150" s="13" t="s">
         <v>607</v>
       </c>
-      <c r="C150" s="12" t="s">
-        <v>608</v>
-      </c>
-      <c r="D150" s="12" t="s">
-        <v>659</v>
+      <c r="C150" t="s">
+        <v>658</v>
+      </c>
+      <c r="D150" t="s">
+        <v>663</v>
       </c>
       <c r="E150" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="F150">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G150"/>
-      <c r="H150" s="13" t="s">
-        <v>126</v>
-      </c>
+      <c r="H150" s="13"/>
       <c r="I150" t="s">
-        <v>49</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J150"/>
       <c r="K150" t="s">
-        <v>85</v>
-      </c>
-      <c r="M150" s="12" t="s">
-        <v>620</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="L150"/>
+      <c r="M150" s="11"/>
+      <c r="N150" t="s">
+        <v>690</v>
+      </c>
+      <c r="O150"/>
+      <c r="P150"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" s="13">
@@ -8616,16 +8623,20 @@
         <v>607</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D151" s="12" t="s">
-        <v>661</v>
-      </c>
-      <c r="E151" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F151" s="12" t="s">
-        <v>211</v>
+        <v>659</v>
+      </c>
+      <c r="E151" t="s">
+        <v>226</v>
+      </c>
+      <c r="F151">
+        <v>8</v>
+      </c>
+      <c r="G151"/>
+      <c r="H151" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="I151" t="s">
         <v>49</v>
@@ -8634,7 +8645,7 @@
         <v>85</v>
       </c>
       <c r="M151" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.3">
@@ -8645,16 +8656,16 @@
         <v>607</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>660</v>
-      </c>
-      <c r="E152" t="s">
-        <v>226</v>
-      </c>
-      <c r="F152">
-        <v>8</v>
+        <v>661</v>
+      </c>
+      <c r="E152" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F152" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="I152" t="s">
         <v>49</v>
@@ -8663,7 +8674,7 @@
         <v>85</v>
       </c>
       <c r="M152" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.3">
@@ -8674,10 +8685,10 @@
         <v>607</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E153" t="s">
         <v>226</v>
@@ -8685,10 +8696,6 @@
       <c r="F153">
         <v>8</v>
       </c>
-      <c r="G153"/>
-      <c r="H153" s="13" t="s">
-        <v>126</v>
-      </c>
       <c r="I153" t="s">
         <v>49</v>
       </c>
@@ -8696,7 +8703,7 @@
         <v>85</v>
       </c>
       <c r="M153" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.3">
@@ -8707,16 +8714,20 @@
         <v>607</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>662</v>
-      </c>
-      <c r="E154" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F154" s="12" t="s">
-        <v>211</v>
+        <v>663</v>
+      </c>
+      <c r="E154" t="s">
+        <v>226</v>
+      </c>
+      <c r="F154">
+        <v>8</v>
+      </c>
+      <c r="G154"/>
+      <c r="H154" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="I154" t="s">
         <v>49</v>
@@ -8725,7 +8736,7 @@
         <v>85</v>
       </c>
       <c r="M154" s="12" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.3">
@@ -8736,16 +8747,16 @@
         <v>607</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>664</v>
-      </c>
-      <c r="E155" t="s">
-        <v>226</v>
-      </c>
-      <c r="F155">
-        <v>8</v>
+        <v>662</v>
+      </c>
+      <c r="E155" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F155" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="I155" t="s">
         <v>49</v>
@@ -8754,7 +8765,7 @@
         <v>85</v>
       </c>
       <c r="M155" s="12" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.3">
@@ -8765,10 +8776,10 @@
         <v>607</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E156" t="s">
         <v>226</v>
@@ -8783,7 +8794,7 @@
         <v>85</v>
       </c>
       <c r="M156" s="12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.3">
@@ -8794,16 +8805,16 @@
         <v>607</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E157" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="F157">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I157" t="s">
         <v>49</v>
@@ -8812,7 +8823,7 @@
         <v>85</v>
       </c>
       <c r="M157" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.3">
@@ -8823,20 +8834,16 @@
         <v>607</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E158" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="F158">
-        <v>8</v>
-      </c>
-      <c r="G158"/>
-      <c r="H158" s="13" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="I158" t="s">
         <v>49</v>
@@ -8845,7 +8852,7 @@
         <v>85</v>
       </c>
       <c r="M158" s="12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.3">
@@ -8856,16 +8863,20 @@
         <v>607</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>668</v>
-      </c>
-      <c r="E159" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F159" s="12" t="s">
-        <v>211</v>
+        <v>667</v>
+      </c>
+      <c r="E159" t="s">
+        <v>226</v>
+      </c>
+      <c r="F159">
+        <v>8</v>
+      </c>
+      <c r="G159"/>
+      <c r="H159" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="I159" t="s">
         <v>49</v>
@@ -8874,7 +8885,7 @@
         <v>85</v>
       </c>
       <c r="M159" s="12" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.3">
@@ -8885,10 +8896,10 @@
         <v>607</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>368</v>
+        <v>617</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E160" s="12" t="s">
         <v>84</v>
@@ -8903,7 +8914,7 @@
         <v>85</v>
       </c>
       <c r="M160" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.3">
@@ -8914,10 +8925,10 @@
         <v>607</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>618</v>
+        <v>368</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E161" s="12" t="s">
         <v>84</v>
@@ -8932,7 +8943,7 @@
         <v>85</v>
       </c>
       <c r="M161" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.3">
@@ -8943,16 +8954,16 @@
         <v>607</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E162" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F162" s="12" t="s">
-        <v>673</v>
+        <v>211</v>
       </c>
       <c r="I162" t="s">
         <v>49</v>
@@ -8961,7 +8972,7 @@
         <v>85</v>
       </c>
       <c r="M162" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.3">
@@ -8972,10 +8983,10 @@
         <v>607</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E163" s="12" t="s">
         <v>84</v>
@@ -8990,6 +9001,35 @@
         <v>85</v>
       </c>
       <c r="M163" s="12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A164" s="13">
+        <v>43</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>607</v>
+      </c>
+      <c r="C164" s="12" t="s">
+        <v>648</v>
+      </c>
+      <c r="D164" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F164" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="I164" t="s">
+        <v>49</v>
+      </c>
+      <c r="K164" t="s">
+        <v>85</v>
+      </c>
+      <c r="M164" s="12" t="s">
         <v>633</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#112: safety_specs - correct ADVS Dataset line 65
</commit_message>
<xml_diff>
--- a/metadata/safety_specs.xlsx
+++ b/metadata/safety_specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny.Gautier\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A89EF14-80C5-45B6-9F82-86D5F31B877C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A063C20B-47FA-426E-A1CB-54C3717EE6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28770" windowHeight="14505" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -2982,11 +2982,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P164"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D140" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5004,7 +5004,7 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C65" t="s">
         <v>235</v>
@@ -10407,8 +10407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>

</xml_diff>